<commit_message>
Cleaned file and data
</commit_message>
<xml_diff>
--- a/nickwork/export2016.xlsx
+++ b/nickwork/export2016.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10909"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickrad/Desktop/workspace/practice/project2/project-baseball/nickwork/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28790E50-10E4-EB4D-84E6-F056A8FD95F1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="460" windowWidth="20960" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>IP</t>
   </si>
@@ -116,16 +110,13 @@
   </si>
   <si>
     <t>Washington-NL</t>
-  </si>
-  <si>
-    <t>Wins</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,14 +179,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -242,7 +225,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -274,27 +257,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,24 +291,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -519,357 +466,259 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>966.1</v>
       </c>
-      <c r="C2">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>845.2</v>
       </c>
-      <c r="C3">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>974.90000000000009</v>
-      </c>
-      <c r="C4">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>974.9000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>946.5</v>
       </c>
-      <c r="C5">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>831.60000000000014</v>
-      </c>
-      <c r="C6">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>831.6000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>1030.8</v>
       </c>
-      <c r="C7">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>997.30000000000018</v>
-      </c>
-      <c r="C8">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>997.3000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>1038.5</v>
       </c>
-      <c r="C9">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>1041.9000000000001</v>
-      </c>
-      <c r="C10">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1041.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11">
         <v>1018.8</v>
       </c>
-      <c r="C11">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12">
         <v>997.9</v>
       </c>
-      <c r="C12">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>1053.9000000000001</v>
-      </c>
-      <c r="C13">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1053.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <v>562.9</v>
       </c>
-      <c r="C14">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15">
         <v>829.1</v>
       </c>
-      <c r="C15">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16">
-        <v>879.90000000000009</v>
-      </c>
-      <c r="C16">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>879.9000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17">
-        <v>918.50000000000011</v>
-      </c>
-      <c r="C17">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>918.5000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>731.5</v>
       </c>
-      <c r="C18">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B19">
-        <v>889.09999999999991</v>
-      </c>
-      <c r="C19">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>889.0999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>1001.2</v>
       </c>
-      <c r="C20">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21">
-        <v>832.90000000000009</v>
-      </c>
-      <c r="C21">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>832.9000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B22">
-        <v>901.80000000000007</v>
-      </c>
-      <c r="C22">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>901.8000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B23">
-        <v>700.90000000000009</v>
-      </c>
-      <c r="C23">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>700.9000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <v>329.6</v>
       </c>
-      <c r="C24">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B25">
-        <v>956.80000000000007</v>
-      </c>
-      <c r="C25">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>956.8000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B26">
-        <v>793.90000000000009</v>
-      </c>
-      <c r="C26">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>793.9000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B27">
         <v>965.9</v>
       </c>
-      <c r="C27">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B28">
-        <v>905.90000000000009</v>
-      </c>
-      <c r="C28">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+        <v>905.9000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29">
-        <v>945.30000000000018</v>
-      </c>
-      <c r="C29">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+        <v>945.3000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B30">
         <v>936.2</v>
       </c>
-      <c r="C30">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B31">
-        <v>1032.5999999999999</v>
-      </c>
-      <c r="C31">
-        <v>95</v>
+        <v>1032.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>